<commit_message>
Small changes to ResearchStudy column descriptions
LF-1896
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Projects\fhir-obs-viewer\src\conf\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F5C240-7B94-4B62-BEFB-1A21B12B7B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE715AD5-108D-42EB-B396-90C7DB80F60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10903,81 +10903,79 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8" t="s">
         <v>475</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="C14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>476</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F14" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8" t="s">
+      <c r="G14" s="8"/>
+      <c r="H14" s="8" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="C15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="7" t="s">
+      <c r="E15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10" t="s">
+      <c r="G15" s="6"/>
+      <c r="H15" s="6" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10" t="s">
-        <v>479</v>
+        <v>44</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>19</v>
@@ -10987,160 +10985,162 @@
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8" t="s">
         <v>481</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="8" t="s">
+      <c r="C18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>482</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F18" s="12" t="s">
         <v>483</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8" t="s">
+      <c r="G18" s="8"/>
+      <c r="H18" s="8" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="C19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="7" t="s">
+      <c r="E19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6" t="s">
+      <c r="G19" s="6"/>
+      <c r="H19" s="6" t="s">
         <v>485</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>486</v>
-      </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10" t="s">
-        <v>488</v>
+        <v>133</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>489</v>
+        <v>15</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>486</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="C22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="7" t="s">
+      <c r="E22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>493</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10" t="s">
+      <c r="G22" s="6"/>
+      <c r="H22" s="6" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="10" t="s">
-        <v>67</v>
+        <v>491</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>68</v>
+        <v>493</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="H23" s="10" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
@@ -11176,7 +11176,7 @@
         <v>70</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Removed all Observation search parameters with 'value' in the name for our server and dbGap server
LF-1896
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Projects\fhir-obs-viewer\src\conf\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B74139F-D2D7-40B2-85DE-0A8F1E332021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA16002B-A3AE-443E-A239-FCA38C43380A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12211,7 +12211,7 @@
         <v>572</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>168</v>
@@ -12233,7 +12233,7 @@
         <v>574</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>168</v>
@@ -12255,7 +12255,7 @@
         <v>576</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>168</v>
@@ -12277,7 +12277,7 @@
         <v>578</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>168</v>
@@ -12321,7 +12321,7 @@
         <v>582</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>168</v>
@@ -12343,7 +12343,7 @@
         <v>584</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>168</v>
@@ -12387,7 +12387,7 @@
         <v>588</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>40</v>
@@ -12409,7 +12409,7 @@
         <v>590</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>272</v>
@@ -12475,7 +12475,7 @@
         <v>597</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>168</v>
@@ -12497,7 +12497,7 @@
         <v>599</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>168</v>
@@ -12541,7 +12541,7 @@
         <v>603</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>40</v>
@@ -12563,7 +12563,7 @@
         <v>605</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>272</v>
@@ -13331,7 +13331,7 @@
         <v>659</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>40</v>
@@ -13353,7 +13353,7 @@
         <v>661</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>23</v>
@@ -13375,7 +13375,7 @@
         <v>663</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F74" s="7" t="s">
         <v>272</v>
@@ -13397,7 +13397,7 @@
         <v>665</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
service base url is not fixed
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions.xlsx
@@ -10453,7 +10453,7 @@
         <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="F20" t="s">
         <v>39</v>
@@ -10581,7 +10581,7 @@
         <v>480</v>
       </c>
       <c r="E26" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="F26" t="s">
         <v>39</v>
@@ -10643,7 +10643,7 @@
         <v>502</v>
       </c>
       <c r="E29" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="F29" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
keep address and name rows
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions.xlsx
@@ -11610,7 +11610,7 @@
         <v>587</v>
       </c>
       <c r="E348" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F348" t="s">
         <v>27</v>
@@ -11652,7 +11652,7 @@
         <v>591</v>
       </c>
       <c r="E350" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F350" t="s">
         <v>27</v>
@@ -11672,7 +11672,7 @@
         <v>593</v>
       </c>
       <c r="E351" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F351" t="s">
         <v>27</v>
@@ -11692,7 +11692,7 @@
         <v>595</v>
       </c>
       <c r="E352" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F352" t="s">
         <v>27</v>
@@ -11712,7 +11712,7 @@
         <v>597</v>
       </c>
       <c r="E353" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F353" t="s">
         <v>27</v>
@@ -11920,7 +11920,7 @@
         <v>623</v>
       </c>
       <c r="E363" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F363" t="s">
         <v>27</v>
@@ -12024,7 +12024,7 @@
         <v>634</v>
       </c>
       <c r="E368" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F368" t="s">
         <v>27</v>
@@ -12256,7 +12256,7 @@
         <v>653</v>
       </c>
       <c r="E379" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F379" t="s">
         <v>27</v>
@@ -12793,7 +12793,7 @@
         <v>69</v>
       </c>
       <c r="E27" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F27" t="s">
         <v>70</v>
@@ -12835,7 +12835,7 @@
         <v>698</v>
       </c>
       <c r="E29" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F29" t="s">
         <v>40</v>
@@ -13453,7 +13453,7 @@
         <v>176</v>
       </c>
       <c r="E57" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F57" t="s">
         <v>53</v>
@@ -13666,7 +13666,7 @@
         <v>482</v>
       </c>
       <c r="E68" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F68" t="s">
         <v>168</v>
@@ -13746,7 +13746,7 @@
         <v>490</v>
       </c>
       <c r="E72" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F72" t="s">
         <v>40</v>
@@ -14873,7 +14873,7 @@
         <v>587</v>
       </c>
       <c r="E127" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F127" t="s">
         <v>27</v>
@@ -14915,7 +14915,7 @@
         <v>591</v>
       </c>
       <c r="E129" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F129" t="s">
         <v>27</v>
@@ -14935,7 +14935,7 @@
         <v>593</v>
       </c>
       <c r="E130" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F130" t="s">
         <v>27</v>
@@ -14955,7 +14955,7 @@
         <v>595</v>
       </c>
       <c r="E131" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F131" t="s">
         <v>27</v>
@@ -14975,7 +14975,7 @@
         <v>597</v>
       </c>
       <c r="E132" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F132" t="s">
         <v>27</v>
@@ -14995,7 +14995,7 @@
         <v>599</v>
       </c>
       <c r="E133" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F133" t="s">
         <v>53</v>
@@ -15183,7 +15183,7 @@
         <v>623</v>
       </c>
       <c r="E142" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F142" t="s">
         <v>27</v>
@@ -15225,7 +15225,7 @@
         <v>625</v>
       </c>
       <c r="E144" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F144" t="s">
         <v>53</v>
@@ -15287,7 +15287,7 @@
         <v>634</v>
       </c>
       <c r="E147" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F147" t="s">
         <v>27</v>
@@ -15519,7 +15519,7 @@
         <v>653</v>
       </c>
       <c r="E158" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F158" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
retry request on 429
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions.xlsx
@@ -12645,7 +12645,7 @@
         <v>44</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F20" t="s">
         <v>40</v>
@@ -12793,7 +12793,7 @@
         <v>69</v>
       </c>
       <c r="E27" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F27" t="s">
         <v>70</v>
@@ -12835,7 +12835,7 @@
         <v>698</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F29" t="s">
         <v>40</v>
@@ -13453,7 +13453,7 @@
         <v>176</v>
       </c>
       <c r="E57" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F57" t="s">
         <v>53</v>
@@ -13666,7 +13666,7 @@
         <v>482</v>
       </c>
       <c r="E68" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F68" t="s">
         <v>168</v>
@@ -13746,7 +13746,7 @@
         <v>490</v>
       </c>
       <c r="E72" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F72" t="s">
         <v>40</v>
@@ -14724,7 +14724,7 @@
         <v>571</v>
       </c>
       <c r="E119" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F119" t="s">
         <v>40</v>
@@ -15121,7 +15121,7 @@
         <v>614</v>
       </c>
       <c r="E139" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F139" t="s">
         <v>358</v>

</xml_diff>

<commit_message>
hide 'value-' search parameters
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions.xlsx
@@ -10403,7 +10403,7 @@
         <v>482</v>
       </c>
       <c r="E289" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F289" t="s">
         <v>168</v>
@@ -10503,7 +10503,7 @@
         <v>492</v>
       </c>
       <c r="E294" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F294" t="s">
         <v>168</v>
@@ -10563,7 +10563,7 @@
         <v>498</v>
       </c>
       <c r="E297" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F297" t="s">
         <v>40</v>
@@ -10645,7 +10645,7 @@
         <v>507</v>
       </c>
       <c r="E301" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F301" t="s">
         <v>168</v>
@@ -11461,7 +11461,7 @@
         <v>571</v>
       </c>
       <c r="E340" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F340" t="s">
         <v>40</v>
@@ -13666,7 +13666,7 @@
         <v>482</v>
       </c>
       <c r="E68" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F68" t="s">
         <v>168</v>
@@ -13766,7 +13766,7 @@
         <v>492</v>
       </c>
       <c r="E73" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F73" t="s">
         <v>168</v>
@@ -13826,7 +13826,7 @@
         <v>498</v>
       </c>
       <c r="E76" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F76" t="s">
         <v>40</v>
@@ -14724,7 +14724,7 @@
         <v>571</v>
       </c>
       <c r="E119" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F119" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
move "variable name" to top
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24603"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3A4EBF8-ACD9-4936-8D6D-23DC167657DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6099DE4F-478A-4D70-ACB8-0B8D8BFF1E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources on LForms server" sheetId="1" r:id="rId1"/>
@@ -1449,6 +1449,15 @@
     <t>Observation</t>
   </si>
   <si>
+    <t>code text</t>
+  </si>
+  <si>
+    <t>variable name</t>
+  </si>
+  <si>
+    <t>The display text associated with the code of the observation type</t>
+  </si>
+  <si>
     <t>Reference to the service request.</t>
   </si>
   <si>
@@ -1468,15 +1477,6 @@
   </si>
   <si>
     <t>The code of the observation type</t>
-  </si>
-  <si>
-    <t>code text</t>
-  </si>
-  <si>
-    <t>variable name</t>
-  </si>
-  <si>
-    <t>The display text associated with the code of the observation type</t>
   </si>
   <si>
     <t>code-value-concept</t>
@@ -4918,8 +4918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H385"/>
   <sheetViews>
-    <sheetView topLeftCell="A259" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D289" sqref="D289"/>
+    <sheetView tabSelected="1" topLeftCell="A269" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A289" sqref="A289:XFD289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10557,170 +10557,170 @@
       </c>
     </row>
     <row r="281" spans="1:8">
-      <c r="B281" t="s">
+      <c r="A281" s="2"/>
+      <c r="B281" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D281" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E281" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F281" s="2"/>
+      <c r="G281" s="2"/>
+      <c r="H281" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8">
+      <c r="B282" t="s">
         <v>188</v>
       </c>
-      <c r="C281" t="s">
-        <v>18</v>
-      </c>
-      <c r="D281" t="s">
+      <c r="C282" t="s">
+        <v>18</v>
+      </c>
+      <c r="D282" t="s">
         <v>188</v>
       </c>
-      <c r="E281" t="s">
-        <v>19</v>
-      </c>
-      <c r="F281" t="s">
+      <c r="E282" t="s">
+        <v>19</v>
+      </c>
+      <c r="F282" t="s">
         <v>35</v>
       </c>
-      <c r="H281" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="282" spans="1:8">
-      <c r="A282" s="4"/>
-      <c r="B282" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="C282" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D282" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E282" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F282" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G282" s="4"/>
-      <c r="H282" s="4" t="s">
-        <v>474</v>
+      <c r="H282" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="283" spans="1:8">
       <c r="A283" s="4"/>
       <c r="B283" s="4" t="s">
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="C283" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D283" s="4" t="s">
-        <v>43</v>
+        <v>191</v>
       </c>
       <c r="E283" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F283" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G283" s="4"/>
       <c r="H283" s="4" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="284" spans="1:8">
-      <c r="A284" s="3"/>
-      <c r="B284" s="3" t="s">
+      <c r="A284" s="4"/>
+      <c r="B284" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C284" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D284" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E284" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F284" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G284" s="4"/>
+      <c r="H284" s="4" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8">
+      <c r="A285" s="3"/>
+      <c r="B285" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C284" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D284" s="3" t="s">
+      <c r="C285" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D285" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E284" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F284" s="3" t="s">
+      <c r="E285" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F285" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G284" s="3"/>
-      <c r="H284" s="3" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="285" spans="1:8">
-      <c r="B285" t="s">
+      <c r="G285" s="3"/>
+      <c r="H285" s="3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8">
+      <c r="B286" t="s">
         <v>44</v>
       </c>
-      <c r="C285" t="s">
-        <v>18</v>
-      </c>
-      <c r="D285" t="s">
+      <c r="C286" t="s">
+        <v>18</v>
+      </c>
+      <c r="D286" t="s">
         <v>44</v>
       </c>
-      <c r="E285" t="s">
-        <v>23</v>
-      </c>
-      <c r="F285" t="s">
+      <c r="E286" t="s">
+        <v>23</v>
+      </c>
+      <c r="F286" t="s">
         <v>40</v>
       </c>
-      <c r="H285" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="286" spans="1:8">
-      <c r="A286" s="3"/>
-      <c r="B286" s="3" t="s">
+      <c r="H286" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8">
+      <c r="A287" s="3"/>
+      <c r="B287" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C286" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D286" s="3" t="s">
+      <c r="C287" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D287" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E286" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F286" s="3" t="s">
+      <c r="E287" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F287" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G286" s="3"/>
-      <c r="H286" s="3" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="287" spans="1:8">
-      <c r="B287" t="s">
+      <c r="G287" s="3"/>
+      <c r="H287" s="3" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8">
+      <c r="B288" t="s">
         <v>53</v>
       </c>
-      <c r="C287" t="s">
-        <v>18</v>
-      </c>
-      <c r="D287" t="s">
+      <c r="C288" t="s">
+        <v>18</v>
+      </c>
+      <c r="D288" t="s">
         <v>53</v>
       </c>
-      <c r="E287" t="s">
-        <v>23</v>
-      </c>
-      <c r="F287" t="s">
+      <c r="E288" t="s">
+        <v>23</v>
+      </c>
+      <c r="F288" t="s">
         <v>40</v>
       </c>
-      <c r="H287" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="288" spans="1:8">
-      <c r="A288" s="2"/>
-      <c r="B288" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C288" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D288" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="E288" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F288" s="2"/>
-      <c r="G288" s="2"/>
-      <c r="H288" s="2" t="s">
+      <c r="H288" t="s">
         <v>482</v>
       </c>
     </row>
@@ -12731,7 +12731,7 @@
   <dimension ref="A1:H164"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+      <selection activeCell="A68" sqref="A68:XFD68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13824,170 +13824,170 @@
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="B60" t="s">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="B61" t="s">
         <v>188</v>
       </c>
-      <c r="C60" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="C61" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" t="s">
         <v>188</v>
       </c>
-      <c r="E60" t="s">
-        <v>19</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="E61" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" t="s">
         <v>35</v>
       </c>
-      <c r="H60" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4" t="s">
-        <v>474</v>
+      <c r="H61" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="4"/>
       <c r="B62" s="4" t="s">
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>43</v>
+        <v>191</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3" t="s">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D63" s="3" t="s">
+      <c r="C64" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F63" s="3" t="s">
+      <c r="E64" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="B64" t="s">
+      <c r="G64" s="3"/>
+      <c r="H64" s="3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="B65" t="s">
         <v>44</v>
       </c>
-      <c r="C64" t="s">
-        <v>18</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" t="s">
         <v>44</v>
       </c>
-      <c r="E64" t="s">
-        <v>19</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="E65" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65" t="s">
         <v>40</v>
       </c>
-      <c r="H64" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3" t="s">
+      <c r="H65" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D65" s="3" t="s">
+      <c r="C66" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E65" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F65" s="3" t="s">
+      <c r="E66" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="B66" t="s">
+      <c r="G66" s="3"/>
+      <c r="H66" s="3" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="B67" t="s">
         <v>53</v>
       </c>
-      <c r="C66" t="s">
-        <v>18</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="C67" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" t="s">
         <v>53</v>
       </c>
-      <c r="E66" t="s">
-        <v>23</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="E67" t="s">
+        <v>23</v>
+      </c>
+      <c r="F67" t="s">
         <v>40</v>
       </c>
-      <c r="H66" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2" t="s">
+      <c r="H67" t="s">
         <v>482</v>
       </c>
     </row>
@@ -15997,8 +15997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A827" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D854" sqref="D854"/>
+    <sheetView topLeftCell="A832" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A854" sqref="A854:XFD854"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23238,7 +23238,7 @@
         <v>38</v>
       </c>
       <c r="H375" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="376" spans="1:8">
@@ -23600,7 +23600,7 @@
         <v>35</v>
       </c>
       <c r="H394" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="395" spans="1:8">
@@ -32372,74 +32372,74 @@
       </c>
     </row>
     <row r="846" spans="1:8">
-      <c r="B846" t="s">
-        <v>188</v>
-      </c>
-      <c r="C846" t="s">
-        <v>18</v>
-      </c>
-      <c r="D846" t="s">
-        <v>188</v>
-      </c>
-      <c r="E846" t="s">
-        <v>23</v>
-      </c>
-      <c r="F846" t="s">
-        <v>35</v>
-      </c>
-      <c r="H846" t="s">
+      <c r="A846" s="2"/>
+      <c r="B846" s="2" t="s">
         <v>473</v>
+      </c>
+      <c r="C846" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D846" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E846" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F846" s="2"/>
+      <c r="G846" s="2"/>
+      <c r="H846" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="847" spans="1:8">
       <c r="B847" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C847" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D847" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E847" t="s">
         <v>23</v>
       </c>
       <c r="F847" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H847" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="848" spans="1:8">
       <c r="B848" t="s">
+        <v>190</v>
+      </c>
+      <c r="C848" t="s">
+        <v>30</v>
+      </c>
+      <c r="D848" t="s">
+        <v>191</v>
+      </c>
+      <c r="E848" t="s">
+        <v>23</v>
+      </c>
+      <c r="F848" t="s">
+        <v>38</v>
+      </c>
+      <c r="H848" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="849" spans="2:8">
+      <c r="B849" t="s">
         <v>42</v>
       </c>
-      <c r="C848" t="s">
-        <v>30</v>
-      </c>
-      <c r="D848" t="s">
+      <c r="C849" t="s">
+        <v>30</v>
+      </c>
+      <c r="D849" t="s">
         <v>43</v>
-      </c>
-      <c r="E848" t="s">
-        <v>23</v>
-      </c>
-      <c r="F848" t="s">
-        <v>40</v>
-      </c>
-      <c r="H848" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="849" spans="1:8">
-      <c r="B849" t="s">
-        <v>44</v>
-      </c>
-      <c r="C849" t="s">
-        <v>30</v>
-      </c>
-      <c r="D849" t="s">
-        <v>45</v>
       </c>
       <c r="E849" t="s">
         <v>23</v>
@@ -32448,18 +32448,18 @@
         <v>40</v>
       </c>
       <c r="H849" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="850" spans="1:8">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="850" spans="2:8">
       <c r="B850" t="s">
         <v>44</v>
       </c>
       <c r="C850" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D850" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E850" t="s">
         <v>23</v>
@@ -32468,18 +32468,18 @@
         <v>40</v>
       </c>
       <c r="H850" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="851" spans="1:8">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="851" spans="2:8">
       <c r="B851" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C851" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D851" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E851" t="s">
         <v>23</v>
@@ -32488,18 +32488,18 @@
         <v>40</v>
       </c>
       <c r="H851" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="852" spans="1:8">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="852" spans="2:8">
       <c r="B852" t="s">
         <v>53</v>
       </c>
       <c r="C852" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D852" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E852" t="s">
         <v>23</v>
@@ -32508,30 +32508,30 @@
         <v>40</v>
       </c>
       <c r="H852" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="853" spans="1:8">
-      <c r="A853" s="2"/>
-      <c r="B853" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C853" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D853" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="E853" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F853" s="2"/>
-      <c r="G853" s="2"/>
-      <c r="H853" s="2" t="s">
+    </row>
+    <row r="853" spans="2:8">
+      <c r="B853" t="s">
+        <v>53</v>
+      </c>
+      <c r="C853" t="s">
+        <v>18</v>
+      </c>
+      <c r="D853" t="s">
+        <v>53</v>
+      </c>
+      <c r="E853" t="s">
+        <v>23</v>
+      </c>
+      <c r="F853" t="s">
+        <v>40</v>
+      </c>
+      <c r="H853" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="854" spans="1:8">
+    <row r="854" spans="2:8">
       <c r="B854" t="s">
         <v>483</v>
       </c>
@@ -32551,7 +32551,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="855" spans="1:8">
+    <row r="855" spans="2:8">
       <c r="B855" t="s">
         <v>485</v>
       </c>
@@ -32571,7 +32571,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="856" spans="1:8">
+    <row r="856" spans="2:8">
       <c r="B856" t="s">
         <v>487</v>
       </c>
@@ -32591,7 +32591,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="857" spans="1:8">
+    <row r="857" spans="2:8">
       <c r="B857" t="s">
         <v>489</v>
       </c>
@@ -32611,7 +32611,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="858" spans="1:8">
+    <row r="858" spans="2:8">
       <c r="B858" t="s">
         <v>491</v>
       </c>
@@ -32631,7 +32631,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="859" spans="1:8">
+    <row r="859" spans="2:8">
       <c r="B859" t="s">
         <v>493</v>
       </c>
@@ -32651,7 +32651,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="860" spans="1:8">
+    <row r="860" spans="2:8">
       <c r="B860" t="s">
         <v>495</v>
       </c>
@@ -32671,7 +32671,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="861" spans="1:8">
+    <row r="861" spans="2:8">
       <c r="B861" t="s">
         <v>497</v>
       </c>
@@ -32691,7 +32691,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="862" spans="1:8">
+    <row r="862" spans="2:8">
       <c r="B862" t="s">
         <v>499</v>
       </c>
@@ -32711,7 +32711,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="863" spans="1:8">
+    <row r="863" spans="2:8">
       <c r="B863" t="s">
         <v>501</v>
       </c>
@@ -32731,7 +32731,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="864" spans="1:8">
+    <row r="864" spans="2:8">
       <c r="B864" t="s">
         <v>503</v>
       </c>

</xml_diff>

<commit_message>
update matching next line
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions.xlsx
@@ -4536,7 +4536,7 @@
       <b/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4555,12 +4555,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4571,12 +4565,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf/>
     <xf fontId="1" applyFont="1"/>
     <xf fillId="2" applyFill="1"/>
     <xf fillId="3" applyFill="1"/>
-    <xf fillId="4" applyFill="1"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -4618,7 +4611,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4"/>
+      <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -4974,7 +4967,7 @@
         <v>58</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>38</v>
@@ -5038,7 +5031,7 @@
       <c r="E30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G30" s="3"/>
@@ -5142,7 +5135,7 @@
       <c r="E35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="3" t="s">
         <v>75</v>
       </c>
       <c r="G35" s="3"/>
@@ -5372,7 +5365,7 @@
       <c r="E46" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F46" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G46" s="3"/>
@@ -5412,7 +5405,7 @@
         <v>106</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>38</v>
@@ -5629,7 +5622,7 @@
       <c r="E59" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="F59" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G59" s="3"/>
@@ -5671,7 +5664,7 @@
       <c r="E61" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F61" s="4" t="s">
+      <c r="F61" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G61" s="3"/>
@@ -6125,7 +6118,7 @@
       <c r="E83" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F83" s="4" t="s">
+      <c r="F83" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G83" s="3"/>
@@ -6289,7 +6282,7 @@
         <v>106</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F91" s="3" t="s">
         <v>38</v>
@@ -6548,7 +6541,7 @@
       <c r="E104" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F104" s="4" t="s">
+      <c r="F104" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G104" s="3"/>
@@ -6610,7 +6603,7 @@
       <c r="E107" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F107" s="4" t="s">
+      <c r="F107" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G107" s="3"/>
@@ -6674,7 +6667,7 @@
       <c r="E110" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F110" s="4" t="s">
+      <c r="F110" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G110" s="3"/>
@@ -6800,7 +6793,7 @@
       <c r="E116" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F116" s="4" t="s">
+      <c r="F116" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G116" s="3"/>
@@ -6882,7 +6875,7 @@
       <c r="E120" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F120" s="4" t="s">
+      <c r="F120" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G120" s="3"/>
@@ -7260,7 +7253,7 @@
       <c r="E138" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F138" s="4" t="s">
+      <c r="F138" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G138" s="3"/>
@@ -7280,7 +7273,7 @@
         <v>106</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F139" s="3" t="s">
         <v>38</v>
@@ -7322,7 +7315,7 @@
         <v>180</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F141" s="3" t="s">
         <v>40</v>
@@ -7563,7 +7556,7 @@
       <c r="E153" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F153" s="4" t="s">
+      <c r="F153" s="3" t="s">
         <v>283</v>
       </c>
       <c r="G153" s="3"/>
@@ -7733,7 +7726,7 @@
       <c r="E161" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F161" s="4" t="s">
+      <c r="F161" s="3" t="s">
         <v>75</v>
       </c>
       <c r="G161" s="3"/>
@@ -7797,7 +7790,7 @@
       <c r="E164" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F164" s="4" t="s">
+      <c r="F164" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G164" s="3"/>
@@ -8005,7 +7998,7 @@
         <v>106</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F174" s="3" t="s">
         <v>38</v>
@@ -8049,7 +8042,7 @@
       <c r="E176" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F176" s="4" t="s">
+      <c r="F176" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G176" s="3"/>
@@ -8414,7 +8407,7 @@
       <c r="E194" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F194" s="4" t="s">
+      <c r="F194" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G194" s="3"/>
@@ -8458,7 +8451,7 @@
       <c r="E196" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F196" s="4" t="s">
+      <c r="F196" s="3" t="s">
         <v>283</v>
       </c>
       <c r="G196" s="3"/>
@@ -8838,7 +8831,7 @@
       <c r="E214" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F214" s="4" t="s">
+      <c r="F214" s="3" t="s">
         <v>75</v>
       </c>
       <c r="G214" s="3"/>
@@ -9180,7 +9173,7 @@
         <v>106</v>
       </c>
       <c r="E230" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F230" s="3" t="s">
         <v>38</v>
@@ -9224,7 +9217,7 @@
       <c r="E232" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F232" s="4" t="s">
+      <c r="F232" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G232" s="3"/>
@@ -9549,7 +9542,7 @@
       <c r="E248" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F248" s="4" t="s">
+      <c r="F248" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G248" s="3"/>
@@ -9781,7 +9774,7 @@
       <c r="E259" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F259" s="4" t="s">
+      <c r="F259" s="3" t="s">
         <v>75</v>
       </c>
       <c r="G259" s="3"/>
@@ -9909,7 +9902,7 @@
       <c r="E265" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F265" s="4" t="s">
+      <c r="F265" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G265" s="3"/>
@@ -10141,7 +10134,7 @@
         <v>106</v>
       </c>
       <c r="E276" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F276" s="3" t="s">
         <v>38</v>
@@ -10602,7 +10595,7 @@
       <c r="E299" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F299" s="4" t="s">
+      <c r="F299" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G299" s="3"/>
@@ -11186,7 +11179,7 @@
       <c r="E327" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F327" s="4" t="s">
+      <c r="F327" s="3" t="s">
         <v>75</v>
       </c>
       <c r="G327" s="3"/>
@@ -11312,7 +11305,7 @@
       <c r="E333" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F333" s="4" t="s">
+      <c r="F333" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G333" s="3"/>
@@ -11416,7 +11409,7 @@
         <v>106</v>
       </c>
       <c r="E338" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F338" s="3" t="s">
         <v>38</v>
@@ -11793,7 +11786,7 @@
       <c r="E357" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F357" s="4" t="s">
+      <c r="F357" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G357" s="3"/>
@@ -11815,7 +11808,7 @@
       <c r="E358" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F358" s="4" t="s">
+      <c r="F358" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G358" s="3"/>
@@ -12145,7 +12138,7 @@
       <c r="E374" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F374" s="4" t="s">
+      <c r="F374" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G374" s="3"/>
@@ -12335,7 +12328,7 @@
       <c r="E383" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F383" s="4" t="s">
+      <c r="F383" s="3" t="s">
         <v>667</v>
       </c>
       <c r="G383" s="3"/>
@@ -12355,7 +12348,7 @@
         <v>670</v>
       </c>
       <c r="E384" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F384" s="3" t="s">
         <v>622</v>
@@ -12426,7 +12419,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4"/>
+      <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -12622,7 +12615,7 @@
       <c r="E19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G19" s="3"/>
@@ -12686,7 +12679,7 @@
       <c r="E22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>690</v>
       </c>
       <c r="G22" s="3"/>
@@ -12728,7 +12721,7 @@
       <c r="E24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>693</v>
       </c>
       <c r="G24" s="3"/>
@@ -12918,7 +12911,7 @@
       <c r="E33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F33" s="3" t="s">
         <v>75</v>
       </c>
       <c r="G33" s="3"/>
@@ -13132,7 +13125,7 @@
       <c r="E42" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G42" s="3"/>
@@ -13368,7 +13361,7 @@
       <c r="E53" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="F53" s="3" t="s">
         <v>760</v>
       </c>
       <c r="G53" s="3"/>
@@ -13579,7 +13572,7 @@
         <v>45</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>40</v>
@@ -13865,7 +13858,7 @@
       <c r="E78" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F78" s="4" t="s">
+      <c r="F78" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G78" s="3"/>
@@ -14449,7 +14442,7 @@
       <c r="E106" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F106" s="4" t="s">
+      <c r="F106" s="3" t="s">
         <v>75</v>
       </c>
       <c r="G106" s="3"/>
@@ -14575,7 +14568,7 @@
       <c r="E112" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F112" s="4" t="s">
+      <c r="F112" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G112" s="3"/>
@@ -14637,7 +14630,7 @@
         <v>177</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F115" s="3" t="s">
         <v>53</v>
@@ -14679,7 +14672,7 @@
         <v>106</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F117" s="3" t="s">
         <v>38</v>
@@ -15056,7 +15049,7 @@
       <c r="E136" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F136" s="4" t="s">
+      <c r="F136" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G136" s="3"/>
@@ -15078,7 +15071,7 @@
       <c r="E137" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F137" s="4" t="s">
+      <c r="F137" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G137" s="3"/>
@@ -15408,7 +15401,7 @@
       <c r="E153" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F153" s="4" t="s">
+      <c r="F153" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G153" s="3"/>
@@ -15598,7 +15591,7 @@
       <c r="E162" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F162" s="4" t="s">
+      <c r="F162" s="3" t="s">
         <v>667</v>
       </c>
       <c r="G162" s="3"/>
@@ -15729,7 +15722,7 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H8" t="s">
@@ -15769,7 +15762,7 @@
       <c r="E10" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H10" t="s">
@@ -16768,7 +16761,7 @@
       <c r="E61" t="s">
         <v>19</v>
       </c>
-      <c r="F61" s="4" t="s">
+      <c r="F61" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H61" t="s">
@@ -16793,7 +16786,7 @@
       <c r="E63" t="s">
         <v>19</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="F63" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H63" t="s">
@@ -17390,7 +17383,7 @@
       <c r="E93" t="s">
         <v>19</v>
       </c>
-      <c r="F93" s="4" t="s">
+      <c r="F93" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H93" t="s">
@@ -17872,7 +17865,7 @@
       <c r="E118" t="s">
         <v>19</v>
       </c>
-      <c r="F118" s="4" t="s">
+      <c r="F118" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H118" t="s">
@@ -17892,7 +17885,7 @@
       <c r="E119" t="s">
         <v>19</v>
       </c>
-      <c r="F119" s="4" t="s">
+      <c r="F119" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H119" t="s">
@@ -18494,7 +18487,7 @@
       <c r="E150" t="s">
         <v>19</v>
       </c>
-      <c r="F150" s="4" t="s">
+      <c r="F150" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H150" t="s">
@@ -18614,7 +18607,7 @@
       <c r="E156" t="s">
         <v>19</v>
       </c>
-      <c r="F156" s="4" t="s">
+      <c r="F156" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H156" t="s">
@@ -19179,7 +19172,7 @@
       <c r="E185" t="s">
         <v>19</v>
       </c>
-      <c r="F185" s="4" t="s">
+      <c r="F185" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H185" t="s">
@@ -19316,7 +19309,7 @@
       <c r="E192" t="s">
         <v>19</v>
       </c>
-      <c r="F192" s="4" t="s">
+      <c r="F192" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H192" t="s">
@@ -19336,7 +19329,7 @@
       <c r="E193" t="s">
         <v>19</v>
       </c>
-      <c r="F193" s="4" t="s">
+      <c r="F193" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H193" t="s">
@@ -20018,7 +20011,7 @@
       <c r="E228" t="s">
         <v>19</v>
       </c>
-      <c r="F228" s="4" t="s">
+      <c r="F228" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H228" t="s">
@@ -20098,7 +20091,7 @@
       <c r="E232" t="s">
         <v>19</v>
       </c>
-      <c r="F232" s="4" t="s">
+      <c r="F232" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H232" t="s">
@@ -20800,7 +20793,7 @@
       <c r="E268" t="s">
         <v>19</v>
       </c>
-      <c r="F268" s="4" t="s">
+      <c r="F268" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H268" t="s">
@@ -20880,7 +20873,7 @@
       <c r="E272" t="s">
         <v>19</v>
       </c>
-      <c r="F272" s="4" t="s">
+      <c r="F272" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H272" t="s">
@@ -21585,7 +21578,7 @@
       <c r="E308" t="s">
         <v>19</v>
       </c>
-      <c r="F308" s="4" t="s">
+      <c r="F308" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H308" t="s">
@@ -21682,7 +21675,7 @@
       <c r="E313" t="s">
         <v>19</v>
       </c>
-      <c r="F313" s="4" t="s">
+      <c r="F313" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H313" t="s">
@@ -21902,7 +21895,7 @@
       <c r="E324" t="s">
         <v>19</v>
       </c>
-      <c r="F324" s="4" t="s">
+      <c r="F324" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H324" t="s">
@@ -22484,7 +22477,7 @@
       <c r="E354" t="s">
         <v>19</v>
       </c>
-      <c r="F354" s="4" t="s">
+      <c r="F354" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H354" t="s">
@@ -22524,7 +22517,7 @@
       <c r="E356" t="s">
         <v>19</v>
       </c>
-      <c r="F356" s="4" t="s">
+      <c r="F356" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H356" t="s">
@@ -23046,7 +23039,7 @@
       <c r="E383" t="s">
         <v>19</v>
       </c>
-      <c r="F383" s="4" t="s">
+      <c r="F383" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H383" t="s">
@@ -23648,7 +23641,7 @@
       <c r="E414" t="s">
         <v>19</v>
       </c>
-      <c r="F414" s="4" t="s">
+      <c r="F414" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H414" t="s">
@@ -23728,7 +23721,7 @@
       <c r="E418" t="s">
         <v>19</v>
       </c>
-      <c r="F418" s="4" t="s">
+      <c r="F418" s="3" t="s">
         <v>667</v>
       </c>
       <c r="H418" t="s">
@@ -24250,7 +24243,7 @@
       <c r="E445" t="s">
         <v>19</v>
       </c>
-      <c r="F445" s="4" t="s">
+      <c r="F445" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H445" t="s">
@@ -24595,7 +24588,7 @@
       <c r="E463" t="s">
         <v>19</v>
       </c>
-      <c r="F463" s="4" t="s">
+      <c r="F463" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H463" t="s">
@@ -24635,7 +24628,7 @@
       <c r="E465" t="s">
         <v>19</v>
       </c>
-      <c r="F465" s="4" t="s">
+      <c r="F465" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H465" t="s">
@@ -25072,7 +25065,7 @@
       <c r="E487" t="s">
         <v>19</v>
       </c>
-      <c r="F487" s="4" t="s">
+      <c r="F487" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H487" t="s">
@@ -25477,7 +25470,7 @@
       <c r="E508" t="s">
         <v>19</v>
       </c>
-      <c r="F508" s="4" t="s">
+      <c r="F508" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H508" t="s">
@@ -25537,7 +25530,7 @@
       <c r="E511" t="s">
         <v>19</v>
       </c>
-      <c r="F511" s="4" t="s">
+      <c r="F511" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H511" t="s">
@@ -25597,7 +25590,7 @@
       <c r="E514" t="s">
         <v>19</v>
       </c>
-      <c r="F514" s="4" t="s">
+      <c r="F514" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H514" t="s">
@@ -25714,7 +25707,7 @@
       <c r="E520" t="s">
         <v>19</v>
       </c>
-      <c r="F520" s="4" t="s">
+      <c r="F520" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H520" t="s">
@@ -25794,7 +25787,7 @@
       <c r="E524" t="s">
         <v>19</v>
       </c>
-      <c r="F524" s="4" t="s">
+      <c r="F524" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H524" t="s">
@@ -26154,7 +26147,7 @@
       <c r="E542" t="s">
         <v>19</v>
       </c>
-      <c r="F542" s="4" t="s">
+      <c r="F542" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H542" t="s">
@@ -26798,7 +26791,7 @@
       <c r="E576" t="s">
         <v>19</v>
       </c>
-      <c r="F576" s="4" t="s">
+      <c r="F576" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H576" t="s">
@@ -27018,7 +27011,7 @@
       <c r="E587" t="s">
         <v>19</v>
       </c>
-      <c r="F587" s="4" t="s">
+      <c r="F587" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H587" t="s">
@@ -27063,7 +27056,7 @@
       <c r="E590" t="s">
         <v>19</v>
       </c>
-      <c r="F590" s="4" t="s">
+      <c r="F590" s="3" t="s">
         <v>1220</v>
       </c>
       <c r="H590" t="s">
@@ -27200,7 +27193,7 @@
       <c r="E597" t="s">
         <v>19</v>
       </c>
-      <c r="F597" s="4" t="s">
+      <c r="F597" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H597" t="s">
@@ -27662,7 +27655,7 @@
       <c r="E621" t="s">
         <v>19</v>
       </c>
-      <c r="F621" s="4" t="s">
+      <c r="F621" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H621" t="s">
@@ -27682,7 +27675,7 @@
       <c r="E622" t="s">
         <v>19</v>
       </c>
-      <c r="F622" s="4" t="s">
+      <c r="F622" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H622" t="s">
@@ -27702,7 +27695,7 @@
       <c r="E623" t="s">
         <v>19</v>
       </c>
-      <c r="F623" s="4" t="s">
+      <c r="F623" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H623" t="s">
@@ -27782,7 +27775,7 @@
       <c r="E627" t="s">
         <v>19</v>
       </c>
-      <c r="F627" s="4" t="s">
+      <c r="F627" s="3" t="s">
         <v>693</v>
       </c>
       <c r="H627" t="s">
@@ -28002,7 +27995,7 @@
       <c r="E638" t="s">
         <v>19</v>
       </c>
-      <c r="F638" s="4" t="s">
+      <c r="F638" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H638" t="s">
@@ -28227,7 +28220,7 @@
       <c r="E650" t="s">
         <v>19</v>
       </c>
-      <c r="F650" s="4" t="s">
+      <c r="F650" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H650" t="s">
@@ -28344,7 +28337,7 @@
       <c r="E656" t="s">
         <v>19</v>
       </c>
-      <c r="F656" s="4" t="s">
+      <c r="F656" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H656" t="s">
@@ -28669,7 +28662,7 @@
       <c r="E673" t="s">
         <v>19</v>
       </c>
-      <c r="F673" s="4" t="s">
+      <c r="F673" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H673" t="s">
@@ -29131,7 +29124,7 @@
       <c r="E697" t="s">
         <v>19</v>
       </c>
-      <c r="F697" s="4" t="s">
+      <c r="F697" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H697" t="s">
@@ -29328,7 +29321,7 @@
       <c r="E707" t="s">
         <v>19</v>
       </c>
-      <c r="F707" s="4" t="s">
+      <c r="F707" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H707" t="s">
@@ -29408,7 +29401,7 @@
       <c r="E711" t="s">
         <v>19</v>
       </c>
-      <c r="F711" s="4" t="s">
+      <c r="F711" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H711" t="s">
@@ -29853,7 +29846,7 @@
       <c r="E734" t="s">
         <v>19</v>
       </c>
-      <c r="F734" s="4" t="s">
+      <c r="F734" s="3" t="s">
         <v>283</v>
       </c>
       <c r="H734" t="s">
@@ -30010,7 +30003,7 @@
       <c r="E742" t="s">
         <v>19</v>
       </c>
-      <c r="F742" s="4" t="s">
+      <c r="F742" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H742" t="s">
@@ -30070,7 +30063,7 @@
       <c r="E745" t="s">
         <v>19</v>
       </c>
-      <c r="F745" s="4" t="s">
+      <c r="F745" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H745" t="s">
@@ -30310,7 +30303,7 @@
       <c r="E757" t="s">
         <v>19</v>
       </c>
-      <c r="F757" s="4" t="s">
+      <c r="F757" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H757" t="s">
@@ -30655,7 +30648,7 @@
       <c r="E775" t="s">
         <v>19</v>
       </c>
-      <c r="F775" s="4" t="s">
+      <c r="F775" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H775" t="s">
@@ -30695,7 +30688,7 @@
       <c r="E777" t="s">
         <v>19</v>
       </c>
-      <c r="F777" s="4" t="s">
+      <c r="F777" s="3" t="s">
         <v>283</v>
       </c>
       <c r="H777" t="s">
@@ -31052,7 +31045,7 @@
       <c r="E795" t="s">
         <v>19</v>
       </c>
-      <c r="F795" s="4" t="s">
+      <c r="F795" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H795" t="s">
@@ -31412,7 +31405,7 @@
       <c r="E813" t="s">
         <v>19</v>
       </c>
-      <c r="F813" s="4" t="s">
+      <c r="F813" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H813" t="s">
@@ -31617,7 +31610,7 @@
       <c r="E824" t="s">
         <v>19</v>
       </c>
-      <c r="F824" s="4" t="s">
+      <c r="F824" s="3" t="s">
         <v>283</v>
       </c>
       <c r="H824" t="s">
@@ -31794,7 +31787,7 @@
       <c r="E833" t="s">
         <v>19</v>
       </c>
-      <c r="F833" s="4" t="s">
+      <c r="F833" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H833" t="s">
@@ -32399,7 +32392,7 @@
       <c r="E864" t="s">
         <v>19</v>
       </c>
-      <c r="F864" s="4" t="s">
+      <c r="F864" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H864" t="s">
@@ -32956,7 +32949,7 @@
       <c r="E892" t="s">
         <v>19</v>
       </c>
-      <c r="F892" s="4" t="s">
+      <c r="F892" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H892" t="s">
@@ -33076,7 +33069,7 @@
       <c r="E898" t="s">
         <v>19</v>
       </c>
-      <c r="F898" s="4" t="s">
+      <c r="F898" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H898" t="s">
@@ -33541,7 +33534,7 @@
       <c r="E922" t="s">
         <v>19</v>
       </c>
-      <c r="F922" s="4" t="s">
+      <c r="F922" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H922" t="s">
@@ -33561,7 +33554,7 @@
       <c r="E923" t="s">
         <v>19</v>
       </c>
-      <c r="F923" s="4" t="s">
+      <c r="F923" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H923" t="s">
@@ -33878,7 +33871,7 @@
       <c r="E939" t="s">
         <v>19</v>
       </c>
-      <c r="F939" s="4" t="s">
+      <c r="F939" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H939" t="s">
@@ -34058,7 +34051,7 @@
       <c r="E948" t="s">
         <v>19</v>
       </c>
-      <c r="F948" s="4" t="s">
+      <c r="F948" s="3" t="s">
         <v>667</v>
       </c>
       <c r="H948" t="s">
@@ -34383,7 +34376,7 @@
       <c r="E965" t="s">
         <v>19</v>
       </c>
-      <c r="F965" s="4" t="s">
+      <c r="F965" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H965" t="s">
@@ -34600,7 +34593,7 @@
       <c r="E976" t="s">
         <v>19</v>
       </c>
-      <c r="F976" s="4" t="s">
+      <c r="F976" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H976" t="s">
@@ -34720,7 +34713,7 @@
       <c r="E982" t="s">
         <v>19</v>
       </c>
-      <c r="F982" s="4" t="s">
+      <c r="F982" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H982" t="s">
@@ -35025,7 +35018,7 @@
       <c r="E998" t="s">
         <v>19</v>
       </c>
-      <c r="F998" s="4" t="s">
+      <c r="F998" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H998" t="s">
@@ -35442,7 +35435,7 @@
       <c r="E1019" t="s">
         <v>19</v>
       </c>
-      <c r="F1019" s="4" t="s">
+      <c r="F1019" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H1019" t="s">
@@ -35687,7 +35680,7 @@
       <c r="E1032" t="s">
         <v>19</v>
       </c>
-      <c r="F1032" s="4" t="s">
+      <c r="F1032" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H1032" t="s">
@@ -35767,7 +35760,7 @@
       <c r="E1036" t="s">
         <v>19</v>
       </c>
-      <c r="F1036" s="4" t="s">
+      <c r="F1036" s="3" t="s">
         <v>690</v>
       </c>
       <c r="H1036" t="s">
@@ -35807,7 +35800,7 @@
       <c r="E1038" t="s">
         <v>19</v>
       </c>
-      <c r="F1038" s="4" t="s">
+      <c r="F1038" s="3" t="s">
         <v>693</v>
       </c>
       <c r="H1038" t="s">
@@ -36024,7 +36017,7 @@
       <c r="E1049" t="s">
         <v>19</v>
       </c>
-      <c r="F1049" s="4" t="s">
+      <c r="F1049" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H1049" t="s">
@@ -36044,7 +36037,7 @@
       <c r="E1050" t="s">
         <v>19</v>
       </c>
-      <c r="F1050" s="4" t="s">
+      <c r="F1050" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H1050" t="s">
@@ -36264,7 +36257,7 @@
       <c r="E1061" t="s">
         <v>19</v>
       </c>
-      <c r="F1061" s="4" t="s">
+      <c r="F1061" s="3" t="s">
         <v>760</v>
       </c>
       <c r="H1061" t="s">
@@ -36726,7 +36719,7 @@
       <c r="E1085" t="s">
         <v>19</v>
       </c>
-      <c r="F1085" s="4" t="s">
+      <c r="F1085" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H1085" t="s">
@@ -36846,7 +36839,7 @@
       <c r="E1091" t="s">
         <v>19</v>
       </c>
-      <c r="F1091" s="4" t="s">
+      <c r="F1091" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H1091" t="s">
@@ -37528,7 +37521,7 @@
       <c r="E1126" t="s">
         <v>19</v>
       </c>
-      <c r="F1126" s="4" t="s">
+      <c r="F1126" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H1126" t="s">

</xml_diff>

<commit_message>
hide "code" and "combo-code" in R4
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions.xlsx
@@ -10354,24 +10354,24 @@
       </c>
     </row>
     <row r="287">
-      <c r="A287" s="3"/>
-      <c r="B287" s="3" t="s">
+      <c r="A287" s="4"/>
+      <c r="B287" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C287" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D287" s="3" t="s">
+      <c r="C287" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D287" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E287" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F287" s="3" t="s">
+      <c r="E287" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F287" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G287" s="3"/>
-      <c r="H287" s="3" t="s">
+      <c r="G287" s="4"/>
+      <c r="H287" s="4" t="s">
         <v>481</v>
       </c>
     </row>
@@ -10386,7 +10386,7 @@
         <v>53</v>
       </c>
       <c r="E288" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F288" t="s">
         <v>40</v>
@@ -10486,7 +10486,7 @@
         <v>491</v>
       </c>
       <c r="E293" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F293" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
search all rows within the same resource type
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions.xlsx
@@ -12506,24 +12506,24 @@
       <c r="H13" s="3"/>
     </row>
     <row r="14">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
         <v>676</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="C14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>677</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="E14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3" t="s">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4" t="s">
         <v>678</v>
       </c>
     </row>
@@ -12594,24 +12594,24 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
         <v>682</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="C18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>683</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="E18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3" t="s">
+      <c r="G18" s="4"/>
+      <c r="H18" s="4" t="s">
         <v>684</v>
       </c>
     </row>

</xml_diff>

<commit_message>
do not update 'subject' column show/hide
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions.xlsx
@@ -5408,24 +5408,24 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4" t="s">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D48" s="4" t="s">
+      <c r="C48" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" s="4" t="s">
+      <c r="E48" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4" t="s">
+      <c r="G48" s="3"/>
+      <c r="H48" s="3" t="s">
         <v>88</v>
       </c>
     </row>
@@ -6285,24 +6285,24 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4" t="s">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C91" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D91" s="4" t="s">
+      <c r="C91" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D91" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E91" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F91" s="4" t="s">
+      <c r="E91" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F91" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G91" s="4"/>
-      <c r="H91" s="4" t="s">
+      <c r="G91" s="3"/>
+      <c r="H91" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -7276,24 +7276,24 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="4"/>
-      <c r="B139" s="4" t="s">
+      <c r="A139" s="3"/>
+      <c r="B139" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C139" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D139" s="4" t="s">
+      <c r="C139" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D139" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E139" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F139" s="4" t="s">
+      <c r="E139" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F139" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G139" s="4"/>
-      <c r="H139" s="4" t="s">
+      <c r="G139" s="3"/>
+      <c r="H139" s="3" t="s">
         <v>232</v>
       </c>
     </row>
@@ -8001,24 +8001,24 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="4"/>
-      <c r="B174" s="4" t="s">
+      <c r="A174" s="3"/>
+      <c r="B174" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C174" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D174" s="4" t="s">
+      <c r="C174" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D174" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E174" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F174" s="4" t="s">
+      <c r="E174" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F174" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G174" s="4"/>
-      <c r="H174" s="4" t="s">
+      <c r="G174" s="3"/>
+      <c r="H174" s="3" t="s">
         <v>318</v>
       </c>
     </row>
@@ -9176,24 +9176,24 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" s="4"/>
-      <c r="B230" s="4" t="s">
+      <c r="A230" s="3"/>
+      <c r="B230" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C230" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D230" s="4" t="s">
+      <c r="C230" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D230" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E230" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F230" s="4" t="s">
+      <c r="E230" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F230" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G230" s="4"/>
-      <c r="H230" s="4" t="s">
+      <c r="G230" s="3"/>
+      <c r="H230" s="3" t="s">
         <v>417</v>
       </c>
     </row>
@@ -10137,24 +10137,24 @@
       </c>
     </row>
     <row r="276">
-      <c r="A276" s="4"/>
-      <c r="B276" s="4" t="s">
+      <c r="A276" s="3"/>
+      <c r="B276" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C276" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D276" s="4" t="s">
+      <c r="C276" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D276" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E276" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F276" s="4" t="s">
+      <c r="E276" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F276" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G276" s="4"/>
-      <c r="H276" s="4" t="s">
+      <c r="G276" s="3"/>
+      <c r="H276" s="3" t="s">
         <v>464</v>
       </c>
     </row>
@@ -11412,24 +11412,24 @@
       </c>
     </row>
     <row r="338">
-      <c r="A338" s="4"/>
-      <c r="B338" s="4" t="s">
+      <c r="A338" s="3"/>
+      <c r="B338" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C338" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D338" s="4" t="s">
+      <c r="C338" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D338" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E338" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F338" s="4" t="s">
+      <c r="E338" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F338" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G338" s="4"/>
-      <c r="H338" s="4" t="s">
+      <c r="G338" s="3"/>
+      <c r="H338" s="3" t="s">
         <v>570</v>
       </c>
     </row>
@@ -14675,24 +14675,24 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="4"/>
-      <c r="B117" s="4" t="s">
+      <c r="A117" s="3"/>
+      <c r="B117" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C117" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D117" s="4" t="s">
+      <c r="C117" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D117" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E117" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F117" s="4" t="s">
+      <c r="E117" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F117" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G117" s="4"/>
-      <c r="H117" s="4" t="s">
+      <c r="G117" s="3"/>
+      <c r="H117" s="3" t="s">
         <v>570</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add evidence variable to base server
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24722"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FCBA6CE-4D8F-459C-A473-4B546FA0347E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8786AFC5-126D-4C8F-A56D-9D9869E2481E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9900" uniqueCount="1513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9934" uniqueCount="1513">
   <si>
     <t>- additional custom columns or custom search parameters</t>
   </si>
@@ -2067,6 +2067,24 @@
     <t>The value in any kind of telecom details of the patient</t>
   </si>
   <si>
+    <t>EvidenceVariable</t>
+  </si>
+  <si>
+    <t>Computationally friendly name of the evidence variable</t>
+  </si>
+  <si>
+    <t>The description of the evidence variable</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>The business version of the evidence variable</t>
+  </si>
+  <si>
     <t>Legend</t>
   </si>
   <si>
@@ -2344,24 +2362,6 @@
   </si>
   <si>
     <t>Facility where study activities are conducted</t>
-  </si>
-  <si>
-    <t>EvidenceVariable</t>
-  </si>
-  <si>
-    <t>Computationally friendly name of the evidence variable</t>
-  </si>
-  <si>
-    <t>The description of the evidence variable</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>The business version of the evidence variable</t>
   </si>
   <si>
     <t>List of all available resources. This sheet is used if no custom configuration is provided.</t>
@@ -4955,9 +4955,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H389"/>
+  <dimension ref="A2:H396"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A376" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I391" sqref="I391:I395"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -12833,6 +12835,137 @@
         <v>678</v>
       </c>
     </row>
+    <row r="390" spans="1:8">
+      <c r="A390" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="391" spans="1:8">
+      <c r="A391" s="2"/>
+      <c r="B391" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="C391" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D391" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="E391" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F391" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G391" s="2"/>
+      <c r="H391" s="2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="392" spans="1:8">
+      <c r="B392" t="s">
+        <v>660</v>
+      </c>
+      <c r="C392" t="s">
+        <v>17</v>
+      </c>
+      <c r="D392" t="s">
+        <v>660</v>
+      </c>
+      <c r="E392" t="s">
+        <v>19</v>
+      </c>
+      <c r="F392" t="s">
+        <v>29</v>
+      </c>
+      <c r="H392" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="393" spans="1:8">
+      <c r="A393" s="2"/>
+      <c r="B393" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C393" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D393" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E393" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F393" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G393" s="2"/>
+      <c r="H393" s="2" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="394" spans="1:8">
+      <c r="B394" t="s">
+        <v>135</v>
+      </c>
+      <c r="C394" t="s">
+        <v>17</v>
+      </c>
+      <c r="D394" t="s">
+        <v>135</v>
+      </c>
+      <c r="E394" t="s">
+        <v>19</v>
+      </c>
+      <c r="F394" t="s">
+        <v>29</v>
+      </c>
+      <c r="H394" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="395" spans="1:8">
+      <c r="A395" s="2"/>
+      <c r="B395" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="C395" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D395" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="E395" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F395" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G395" s="2"/>
+      <c r="H395" s="2" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="396" spans="1:8">
+      <c r="B396" t="s">
+        <v>682</v>
+      </c>
+      <c r="C396" t="s">
+        <v>17</v>
+      </c>
+      <c r="D396" t="s">
+        <v>682</v>
+      </c>
+      <c r="E396" t="s">
+        <v>19</v>
+      </c>
+      <c r="F396" t="s">
+        <v>29</v>
+      </c>
+      <c r="H396" t="s">
+        <v>684</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
@@ -12840,10 +12973,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I171"/>
+  <dimension ref="A1:H171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H171" sqref="H171"/>
+    <sheetView tabSelected="1" topLeftCell="H149" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I166" sqref="I166:I170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12859,7 +12992,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="5" t="s">
-        <v>679</v>
+        <v>685</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -12888,7 +13021,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>680</v>
+        <v>686</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -12896,7 +13029,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>681</v>
+        <v>687</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -12927,7 +13060,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>682</v>
+        <v>688</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -12953,13 +13086,13 @@
     <row r="14" spans="1:8">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>684</v>
+        <v>690</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>22</v>
@@ -12969,7 +13102,7 @@
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
-        <v>685</v>
+        <v>691</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -12991,7 +13124,7 @@
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>686</v>
+        <v>692</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -13013,7 +13146,7 @@
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>687</v>
+        <v>693</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -13035,19 +13168,19 @@
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>690</v>
+        <v>696</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>22</v>
@@ -13057,19 +13190,19 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>691</v>
+        <v>697</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>692</v>
+        <v>698</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>693</v>
+        <v>699</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>22</v>
@@ -13079,7 +13212,7 @@
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
-        <v>694</v>
+        <v>700</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -13099,13 +13232,13 @@
         <v>42</v>
       </c>
       <c r="H20" t="s">
-        <v>687</v>
+        <v>693</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>32</v>
@@ -13121,7 +13254,7 @@
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>696</v>
+        <v>702</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -13139,11 +13272,11 @@
         <v>22</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>697</v>
+        <v>703</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>698</v>
+        <v>704</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -13163,7 +13296,7 @@
         <v>92</v>
       </c>
       <c r="H23" t="s">
-        <v>699</v>
+        <v>705</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -13181,23 +13314,23 @@
         <v>22</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>701</v>
+        <v>707</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>702</v>
+        <v>708</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>703</v>
+        <v>709</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>22</v>
@@ -13207,7 +13340,7 @@
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
-        <v>704</v>
+        <v>710</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -13227,7 +13360,7 @@
         <v>42</v>
       </c>
       <c r="H26" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -13247,7 +13380,7 @@
         <v>72</v>
       </c>
       <c r="H27" t="s">
-        <v>705</v>
+        <v>711</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -13269,18 +13402,18 @@
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>705</v>
+        <v>711</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="B29" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="E29" t="s">
         <v>19</v>
@@ -13289,19 +13422,19 @@
         <v>42</v>
       </c>
       <c r="H29" t="s">
-        <v>707</v>
+        <v>713</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>708</v>
+        <v>714</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>19</v>
@@ -13311,7 +13444,7 @@
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>707</v>
+        <v>713</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -13331,7 +13464,7 @@
         <v>42</v>
       </c>
       <c r="H31" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -13353,7 +13486,7 @@
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -13375,211 +13508,211 @@
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>713</v>
+        <v>719</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>714</v>
+        <v>720</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>715</v>
+        <v>721</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>716</v>
+        <v>722</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>717</v>
+        <v>723</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>713</v>
+        <v>719</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>718</v>
+        <v>724</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>719</v>
+        <v>725</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>721</v>
+        <v>727</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>713</v>
+        <v>719</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>722</v>
+        <v>728</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>723</v>
+        <v>729</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>724</v>
+        <v>730</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>725</v>
+        <v>731</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>713</v>
+        <v>719</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>726</v>
+        <v>732</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>727</v>
+        <v>733</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>728</v>
+        <v>734</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>729</v>
+        <v>735</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>713</v>
+        <v>719</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>730</v>
+        <v>736</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>731</v>
+        <v>737</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>732</v>
+        <v>738</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>733</v>
+        <v>739</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>713</v>
+        <v>719</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>734</v>
+        <v>740</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>735</v>
+        <v>741</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>736</v>
+        <v>742</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>737</v>
+        <v>743</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>713</v>
+        <v>719</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>738</v>
+        <v>744</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>739</v>
+        <v>745</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>741</v>
+        <v>747</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>713</v>
+        <v>719</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>742</v>
+        <v>748</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>743</v>
+        <v>749</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>745</v>
+        <v>751</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>22</v>
@@ -13589,18 +13722,18 @@
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3" t="s">
-        <v>746</v>
+        <v>752</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="B43" t="s">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
       </c>
       <c r="D43" t="s">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="E43" t="s">
         <v>22</v>
@@ -13609,7 +13742,7 @@
         <v>37</v>
       </c>
       <c r="H43" t="s">
-        <v>748</v>
+        <v>754</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -13631,7 +13764,7 @@
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3" t="s">
-        <v>748</v>
+        <v>754</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -13653,19 +13786,19 @@
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3" t="s">
-        <v>699</v>
+        <v>705</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
-        <v>749</v>
+        <v>755</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>750</v>
+        <v>756</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>22</v>
@@ -13675,19 +13808,19 @@
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3" t="s">
-        <v>751</v>
+        <v>757</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>753</v>
+        <v>759</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>22</v>
@@ -13697,18 +13830,18 @@
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3" t="s">
-        <v>754</v>
+        <v>760</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="B48" t="s">
-        <v>755</v>
+        <v>761</v>
       </c>
       <c r="C48" t="s">
         <v>17</v>
       </c>
       <c r="D48" t="s">
-        <v>755</v>
+        <v>761</v>
       </c>
       <c r="E48" t="s">
         <v>22</v>
@@ -13717,19 +13850,19 @@
         <v>37</v>
       </c>
       <c r="H48" t="s">
-        <v>756</v>
+        <v>762</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
-        <v>757</v>
+        <v>763</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>758</v>
+        <v>764</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>22</v>
@@ -13739,19 +13872,19 @@
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3" t="s">
-        <v>756</v>
+        <v>762</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="3"/>
       <c r="B50" s="3" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>22</v>
@@ -13761,18 +13894,18 @@
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3" t="s">
-        <v>761</v>
+        <v>767</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="B51" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
       <c r="C51" t="s">
         <v>17</v>
       </c>
       <c r="D51" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
       <c r="E51" t="s">
         <v>22</v>
@@ -13781,19 +13914,19 @@
         <v>37</v>
       </c>
       <c r="H51" t="s">
-        <v>761</v>
+        <v>767</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="3"/>
       <c r="B52" s="3" t="s">
-        <v>762</v>
+        <v>768</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>763</v>
+        <v>769</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>22</v>
@@ -13803,41 +13936,41 @@
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3" t="s">
-        <v>764</v>
+        <v>770</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="3"/>
       <c r="B53" s="3" t="s">
-        <v>765</v>
+        <v>771</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>766</v>
+        <v>772</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3" t="s">
-        <v>768</v>
+        <v>774</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="3"/>
       <c r="B54" s="3" t="s">
-        <v>769</v>
+        <v>775</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>770</v>
+        <v>776</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>22</v>
@@ -13847,18 +13980,18 @@
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3" t="s">
-        <v>771</v>
+        <v>777</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="B55" t="s">
-        <v>769</v>
+        <v>775</v>
       </c>
       <c r="C55" t="s">
         <v>17</v>
       </c>
       <c r="D55" t="s">
-        <v>769</v>
+        <v>775</v>
       </c>
       <c r="E55" t="s">
         <v>22</v>
@@ -13867,18 +14000,18 @@
         <v>37</v>
       </c>
       <c r="H55" t="s">
-        <v>771</v>
+        <v>777</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="B56" t="s">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="C56" t="s">
         <v>17</v>
       </c>
       <c r="D56" t="s">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="E56" t="s">
         <v>22</v>
@@ -13887,7 +14020,7 @@
         <v>37</v>
       </c>
       <c r="H56" t="s">
-        <v>691</v>
+        <v>697</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -13907,18 +14040,18 @@
         <v>55</v>
       </c>
       <c r="H57" t="s">
-        <v>686</v>
+        <v>692</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="B58" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="C58" t="s">
         <v>17</v>
       </c>
       <c r="D58" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="E58" t="s">
         <v>22</v>
@@ -13927,7 +14060,7 @@
         <v>29</v>
       </c>
       <c r="H58" t="s">
-        <v>685</v>
+        <v>691</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -16016,7 +16149,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:8">
       <c r="B161" t="s">
         <v>669</v>
       </c>
@@ -16036,7 +16169,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:8">
       <c r="A162" s="3"/>
       <c r="B162" s="3" t="s">
         <v>671</v>
@@ -16058,7 +16191,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:8">
       <c r="A163" s="3"/>
       <c r="B163" s="3" t="s">
         <v>675</v>
@@ -16080,7 +16213,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:8">
       <c r="B164" t="s">
         <v>675</v>
       </c>
@@ -16100,12 +16233,12 @@
         <v>678</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:8">
       <c r="A165" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8">
       <c r="A166" s="2"/>
       <c r="B166" s="2" t="s">
         <v>660</v>
@@ -16124,13 +16257,10 @@
       </c>
       <c r="G166" s="2"/>
       <c r="H166" s="2" t="s">
-        <v>773</v>
-      </c>
-      <c r="I166" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8">
       <c r="B167" t="s">
         <v>660</v>
       </c>
@@ -16147,10 +16277,10 @@
         <v>29</v>
       </c>
       <c r="H167" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8">
       <c r="A168" s="2"/>
       <c r="B168" s="2" t="s">
         <v>135</v>
@@ -16169,13 +16299,10 @@
       </c>
       <c r="G168" s="2"/>
       <c r="H168" s="2" t="s">
-        <v>774</v>
-      </c>
-      <c r="I168" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8">
       <c r="B169" t="s">
         <v>135</v>
       </c>
@@ -16192,19 +16319,19 @@
         <v>29</v>
       </c>
       <c r="H169" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8">
       <c r="A170" s="2"/>
       <c r="B170" s="2" t="s">
-        <v>775</v>
+        <v>682</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>776</v>
+        <v>683</v>
       </c>
       <c r="E170" s="2" t="s">
         <v>19</v>
@@ -16214,21 +16341,18 @@
       </c>
       <c r="G170" s="2"/>
       <c r="H170" s="2" t="s">
-        <v>777</v>
-      </c>
-      <c r="I170" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8">
       <c r="B171" t="s">
-        <v>775</v>
+        <v>682</v>
       </c>
       <c r="C171" t="s">
         <v>17</v>
       </c>
       <c r="D171" t="s">
-        <v>775</v>
+        <v>682</v>
       </c>
       <c r="E171" t="s">
         <v>19</v>
@@ -16237,7 +16361,7 @@
         <v>29</v>
       </c>
       <c r="H171" t="s">
-        <v>777</v>
+        <v>684</v>
       </c>
     </row>
   </sheetData>
@@ -17617,13 +17741,13 @@
     </row>
     <row r="75" spans="2:8">
       <c r="B75" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="C75" t="s">
         <v>17</v>
       </c>
       <c r="D75" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="E75" t="s">
         <v>19</v>
@@ -18234,13 +18358,13 @@
     </row>
     <row r="106" spans="1:8">
       <c r="B106" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="C106" t="s">
         <v>32</v>
       </c>
       <c r="D106" t="s">
-        <v>684</v>
+        <v>690</v>
       </c>
       <c r="E106" t="s">
         <v>19</v>
@@ -20080,13 +20204,13 @@
     </row>
     <row r="201" spans="2:8">
       <c r="B201" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
       <c r="C201" t="s">
         <v>32</v>
       </c>
       <c r="D201" t="s">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="E201" t="s">
         <v>19</v>
@@ -28378,7 +28502,7 @@
         <v>22</v>
       </c>
       <c r="F627" s="4" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
       <c r="H627" t="s">
         <v>1283</v>
@@ -29128,13 +29252,13 @@
     </row>
     <row r="666" spans="1:8">
       <c r="B666" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="C666" t="s">
         <v>32</v>
       </c>
       <c r="D666" t="s">
-        <v>684</v>
+        <v>690</v>
       </c>
       <c r="E666" t="s">
         <v>19</v>
@@ -29148,13 +29272,13 @@
     </row>
     <row r="667" spans="1:8">
       <c r="B667" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="C667" t="s">
         <v>17</v>
       </c>
       <c r="D667" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="E667" t="s">
         <v>19</v>
@@ -36266,18 +36390,18 @@
     </row>
     <row r="1031" spans="1:8">
       <c r="A1031" t="s">
-        <v>682</v>
+        <v>688</v>
       </c>
     </row>
     <row r="1032" spans="1:8">
       <c r="B1032" t="s">
-        <v>692</v>
+        <v>698</v>
       </c>
       <c r="C1032" t="s">
         <v>32</v>
       </c>
       <c r="D1032" t="s">
-        <v>693</v>
+        <v>699</v>
       </c>
       <c r="E1032" t="s">
         <v>22</v>
@@ -36286,7 +36410,7 @@
         <v>65</v>
       </c>
       <c r="H1032" t="s">
-        <v>694</v>
+        <v>700</v>
       </c>
     </row>
     <row r="1033" spans="1:8">
@@ -36306,7 +36430,7 @@
         <v>42</v>
       </c>
       <c r="H1033" t="s">
-        <v>687</v>
+        <v>693</v>
       </c>
     </row>
     <row r="1034" spans="1:8">
@@ -36326,12 +36450,12 @@
         <v>42</v>
       </c>
       <c r="H1034" t="s">
-        <v>687</v>
+        <v>693</v>
       </c>
     </row>
     <row r="1035" spans="1:8">
       <c r="B1035" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="C1035" t="s">
         <v>32</v>
@@ -36346,7 +36470,7 @@
         <v>42</v>
       </c>
       <c r="H1035" t="s">
-        <v>696</v>
+        <v>702</v>
       </c>
     </row>
     <row r="1036" spans="1:8">
@@ -36363,10 +36487,10 @@
         <v>22</v>
       </c>
       <c r="F1036" s="4" t="s">
-        <v>697</v>
+        <v>703</v>
       </c>
       <c r="H1036" t="s">
-        <v>698</v>
+        <v>704</v>
       </c>
     </row>
     <row r="1037" spans="1:8">
@@ -36386,7 +36510,7 @@
         <v>92</v>
       </c>
       <c r="H1037" t="s">
-        <v>699</v>
+        <v>705</v>
       </c>
     </row>
     <row r="1038" spans="1:8">
@@ -36403,21 +36527,21 @@
         <v>22</v>
       </c>
       <c r="F1038" s="4" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
       <c r="H1038" t="s">
-        <v>701</v>
+        <v>707</v>
       </c>
     </row>
     <row r="1039" spans="1:8">
       <c r="B1039" t="s">
-        <v>702</v>
+        <v>708</v>
       </c>
       <c r="C1039" t="s">
         <v>32</v>
       </c>
       <c r="D1039" t="s">
-        <v>703</v>
+        <v>709</v>
       </c>
       <c r="E1039" t="s">
         <v>19</v>
@@ -36426,7 +36550,7 @@
         <v>40</v>
       </c>
       <c r="H1039" t="s">
-        <v>704</v>
+        <v>710</v>
       </c>
     </row>
     <row r="1040" spans="1:8">
@@ -36446,7 +36570,7 @@
         <v>42</v>
       </c>
       <c r="H1040" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
     <row r="1041" spans="2:8">
@@ -36466,7 +36590,7 @@
         <v>42</v>
       </c>
       <c r="H1041" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
     <row r="1042" spans="2:8">
@@ -36503,7 +36627,7 @@
         <v>72</v>
       </c>
       <c r="H1043" t="s">
-        <v>705</v>
+        <v>711</v>
       </c>
     </row>
     <row r="1044" spans="2:8">
@@ -36523,18 +36647,18 @@
         <v>72</v>
       </c>
       <c r="H1044" t="s">
-        <v>705</v>
+        <v>711</v>
       </c>
     </row>
     <row r="1045" spans="2:8">
       <c r="B1045" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="C1045" t="s">
         <v>17</v>
       </c>
       <c r="D1045" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="E1045" t="s">
         <v>19</v>
@@ -36543,18 +36667,18 @@
         <v>42</v>
       </c>
       <c r="H1045" t="s">
-        <v>707</v>
+        <v>713</v>
       </c>
     </row>
     <row r="1046" spans="2:8">
       <c r="B1046" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="C1046" t="s">
         <v>32</v>
       </c>
       <c r="D1046" t="s">
-        <v>708</v>
+        <v>714</v>
       </c>
       <c r="E1046" t="s">
         <v>19</v>
@@ -36563,7 +36687,7 @@
         <v>42</v>
       </c>
       <c r="H1046" t="s">
-        <v>707</v>
+        <v>713</v>
       </c>
     </row>
     <row r="1047" spans="2:8">
@@ -36583,7 +36707,7 @@
         <v>42</v>
       </c>
       <c r="H1047" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
     </row>
     <row r="1048" spans="2:8">
@@ -36603,7 +36727,7 @@
         <v>42</v>
       </c>
       <c r="H1048" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
     </row>
     <row r="1049" spans="2:8">
@@ -36623,18 +36747,18 @@
         <v>77</v>
       </c>
       <c r="H1049" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
     </row>
     <row r="1050" spans="2:8">
       <c r="B1050" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="C1050" t="s">
         <v>32</v>
       </c>
       <c r="D1050" t="s">
-        <v>745</v>
+        <v>751</v>
       </c>
       <c r="E1050" t="s">
         <v>22</v>
@@ -36643,18 +36767,18 @@
         <v>65</v>
       </c>
       <c r="H1050" t="s">
-        <v>746</v>
+        <v>752</v>
       </c>
     </row>
     <row r="1051" spans="2:8">
       <c r="B1051" t="s">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="C1051" t="s">
         <v>17</v>
       </c>
       <c r="D1051" t="s">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="E1051" t="s">
         <v>19</v>
@@ -36663,7 +36787,7 @@
         <v>37</v>
       </c>
       <c r="H1051" t="s">
-        <v>748</v>
+        <v>754</v>
       </c>
     </row>
     <row r="1052" spans="2:8">
@@ -36683,7 +36807,7 @@
         <v>40</v>
       </c>
       <c r="H1052" t="s">
-        <v>748</v>
+        <v>754</v>
       </c>
     </row>
     <row r="1053" spans="2:8">
@@ -36703,18 +36827,18 @@
         <v>235</v>
       </c>
       <c r="H1053" t="s">
-        <v>699</v>
+        <v>705</v>
       </c>
     </row>
     <row r="1054" spans="2:8">
       <c r="B1054" t="s">
-        <v>749</v>
+        <v>755</v>
       </c>
       <c r="C1054" t="s">
         <v>32</v>
       </c>
       <c r="D1054" t="s">
-        <v>750</v>
+        <v>756</v>
       </c>
       <c r="E1054" t="s">
         <v>19</v>
@@ -36723,18 +36847,18 @@
         <v>42</v>
       </c>
       <c r="H1054" t="s">
-        <v>751</v>
+        <v>757</v>
       </c>
     </row>
     <row r="1055" spans="2:8">
       <c r="B1055" t="s">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c r="C1055" t="s">
         <v>32</v>
       </c>
       <c r="D1055" t="s">
-        <v>753</v>
+        <v>759</v>
       </c>
       <c r="E1055" t="s">
         <v>19</v>
@@ -36743,18 +36867,18 @@
         <v>42</v>
       </c>
       <c r="H1055" t="s">
-        <v>754</v>
+        <v>760</v>
       </c>
     </row>
     <row r="1056" spans="2:8">
       <c r="B1056" t="s">
-        <v>755</v>
+        <v>761</v>
       </c>
       <c r="C1056" t="s">
         <v>17</v>
       </c>
       <c r="D1056" t="s">
-        <v>755</v>
+        <v>761</v>
       </c>
       <c r="E1056" t="s">
         <v>19</v>
@@ -36763,18 +36887,18 @@
         <v>37</v>
       </c>
       <c r="H1056" t="s">
-        <v>756</v>
+        <v>762</v>
       </c>
     </row>
     <row r="1057" spans="1:8">
       <c r="B1057" t="s">
-        <v>757</v>
+        <v>763</v>
       </c>
       <c r="C1057" t="s">
         <v>32</v>
       </c>
       <c r="D1057" t="s">
-        <v>758</v>
+        <v>764</v>
       </c>
       <c r="E1057" t="s">
         <v>19</v>
@@ -36783,18 +36907,18 @@
         <v>40</v>
       </c>
       <c r="H1057" t="s">
-        <v>756</v>
+        <v>762</v>
       </c>
     </row>
     <row r="1058" spans="1:8">
       <c r="B1058" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
       <c r="C1058" t="s">
         <v>32</v>
       </c>
       <c r="D1058" t="s">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="E1058" t="s">
         <v>19</v>
@@ -36803,18 +36927,18 @@
         <v>40</v>
       </c>
       <c r="H1058" t="s">
-        <v>761</v>
+        <v>767</v>
       </c>
     </row>
     <row r="1059" spans="1:8">
       <c r="B1059" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
       <c r="C1059" t="s">
         <v>17</v>
       </c>
       <c r="D1059" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
       <c r="E1059" t="s">
         <v>19</v>
@@ -36823,18 +36947,18 @@
         <v>37</v>
       </c>
       <c r="H1059" t="s">
-        <v>761</v>
+        <v>767</v>
       </c>
     </row>
     <row r="1060" spans="1:8">
       <c r="B1060" t="s">
-        <v>762</v>
+        <v>768</v>
       </c>
       <c r="C1060" t="s">
         <v>32</v>
       </c>
       <c r="D1060" t="s">
-        <v>763</v>
+        <v>769</v>
       </c>
       <c r="E1060" t="s">
         <v>19</v>
@@ -36843,38 +36967,38 @@
         <v>42</v>
       </c>
       <c r="H1060" t="s">
-        <v>764</v>
+        <v>770</v>
       </c>
     </row>
     <row r="1061" spans="1:8">
       <c r="B1061" t="s">
-        <v>765</v>
+        <v>771</v>
       </c>
       <c r="C1061" t="s">
         <v>32</v>
       </c>
       <c r="D1061" t="s">
-        <v>766</v>
+        <v>772</v>
       </c>
       <c r="E1061" t="s">
         <v>22</v>
       </c>
       <c r="F1061" s="4" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="H1061" t="s">
-        <v>768</v>
+        <v>774</v>
       </c>
     </row>
     <row r="1062" spans="1:8">
       <c r="B1062" t="s">
-        <v>769</v>
+        <v>775</v>
       </c>
       <c r="C1062" t="s">
         <v>32</v>
       </c>
       <c r="D1062" t="s">
-        <v>770</v>
+        <v>776</v>
       </c>
       <c r="E1062" t="s">
         <v>19</v>
@@ -36883,18 +37007,18 @@
         <v>40</v>
       </c>
       <c r="H1062" t="s">
-        <v>771</v>
+        <v>777</v>
       </c>
     </row>
     <row r="1063" spans="1:8">
       <c r="B1063" t="s">
-        <v>769</v>
+        <v>775</v>
       </c>
       <c r="C1063" t="s">
         <v>17</v>
       </c>
       <c r="D1063" t="s">
-        <v>769</v>
+        <v>775</v>
       </c>
       <c r="E1063" t="s">
         <v>19</v>
@@ -36903,18 +37027,18 @@
         <v>37</v>
       </c>
       <c r="H1063" t="s">
-        <v>771</v>
+        <v>777</v>
       </c>
     </row>
     <row r="1064" spans="1:8">
       <c r="B1064" t="s">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="C1064" t="s">
         <v>32</v>
       </c>
       <c r="D1064" t="s">
-        <v>690</v>
+        <v>696</v>
       </c>
       <c r="E1064" t="s">
         <v>19</v>
@@ -36923,18 +37047,18 @@
         <v>40</v>
       </c>
       <c r="H1064" t="s">
-        <v>691</v>
+        <v>697</v>
       </c>
     </row>
     <row r="1065" spans="1:8">
       <c r="B1065" t="s">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="C1065" t="s">
         <v>17</v>
       </c>
       <c r="D1065" t="s">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="E1065" t="s">
         <v>19</v>
@@ -36943,7 +37067,7 @@
         <v>37</v>
       </c>
       <c r="H1065" t="s">
-        <v>691</v>
+        <v>697</v>
       </c>
     </row>
     <row r="1066" spans="1:8">
@@ -36963,7 +37087,7 @@
         <v>55</v>
       </c>
       <c r="H1066" t="s">
-        <v>686</v>
+        <v>692</v>
       </c>
     </row>
     <row r="1067" spans="1:8">
@@ -36983,18 +37107,18 @@
         <v>55</v>
       </c>
       <c r="H1067" t="s">
-        <v>686</v>
+        <v>692</v>
       </c>
     </row>
     <row r="1068" spans="1:8">
       <c r="B1068" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="C1068" t="s">
         <v>17</v>
       </c>
       <c r="D1068" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="E1068" t="s">
         <v>19</v>
@@ -37003,18 +37127,18 @@
         <v>29</v>
       </c>
       <c r="H1068" t="s">
-        <v>685</v>
+        <v>691</v>
       </c>
     </row>
     <row r="1069" spans="1:8">
       <c r="B1069" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="C1069" t="s">
         <v>32</v>
       </c>
       <c r="D1069" t="s">
-        <v>684</v>
+        <v>690</v>
       </c>
       <c r="E1069" t="s">
         <v>19</v>
@@ -37023,7 +37147,7 @@
         <v>29</v>
       </c>
       <c r="H1069" t="s">
-        <v>685</v>
+        <v>691</v>
       </c>
     </row>
     <row r="1070" spans="1:8">
@@ -37093,13 +37217,13 @@
     </row>
     <row r="1074" spans="2:8">
       <c r="B1074" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="C1074" t="s">
         <v>17</v>
       </c>
       <c r="D1074" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="E1074" t="s">
         <v>19</v>
@@ -37113,7 +37237,7 @@
     </row>
     <row r="1075" spans="2:8">
       <c r="B1075" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="C1075" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
keep value[x] column shown
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions.xlsx
@@ -11642,7 +11642,7 @@
         <v>587</v>
       </c>
       <c r="E348" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F348" s="3" t="s">
         <v>588</v>
@@ -14905,7 +14905,7 @@
         <v>587</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F123" s="3" t="s">
         <v>588</v>

</xml_diff>